<commit_message>
vendor/customer import file updated (#1rp6hyz)
</commit_message>
<xml_diff>
--- a/public/files/import/vendors.xlsx
+++ b/public/files/import/vendors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7070"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="vendors" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
@@ -31,6 +31,18 @@
     <t>address</t>
   </si>
   <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zip_code</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
     <t>website</t>
   </si>
   <si>
@@ -50,6 +62,9 @@
   </si>
   <si>
     <t>test@vendor.com</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
   <si>
     <t>USD</t>
@@ -60,10 +75,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -74,50 +89,106 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -131,24 +202,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -156,69 +225,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,13 +248,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,169 +416,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,11 +442,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -451,13 +472,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -480,32 +514,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -530,145 +545,145 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1022,25 +1037,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="18.7090909090909" customWidth="1"/>
-    <col min="3" max="3" width="12.8545454545455" customWidth="1"/>
+    <col min="2" max="2" width="18.712962962963" customWidth="1"/>
+    <col min="3" max="3" width="12.8518518518519" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="6" width="9.28181818181818" customWidth="1"/>
-    <col min="7" max="7" width="16.4272727272727" customWidth="1"/>
-    <col min="8" max="8" width="11.7090909090909" customWidth="1"/>
-    <col min="9" max="10" width="9.28181818181818" customWidth="1"/>
+    <col min="5" max="6" width="9.27777777777778" customWidth="1"/>
+    <col min="7" max="7" width="16.4259259259259" customWidth="1"/>
+    <col min="8" max="8" width="11.712962962963" customWidth="1"/>
+    <col min="9" max="10" width="9.27777777777778" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1071,18 +1086,34 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="b">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2"/>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>